<commit_message>
07212020 Nevada Water Allocations Upload
07212020 Nevada Water Allocations Upload.  Joseph mapped.  Need a few corrections on mispelling and labeling.
</commit_message>
<xml_diff>
--- a/Nevada/WaterAllocation/NV_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Nevada/WaterAllocation/NV_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustus/Desktop/WSWC/WaDE/MappingStatesDataToWaDE2.0/Nevada/WaterAllocation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Nevada\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9708937-7798-284E-B564-E0219C986B23}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BB6AD9-6048-4E79-BA9E-E0D658AFDA9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34280" yWindow="460" windowWidth="32060" windowHeight="18240" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="714" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -30,6 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="287">
   <si>
     <t>AllocationAmount</t>
   </si>
@@ -883,6 +886,21 @@
   </si>
   <si>
     <t>bmcmenamy@water.nv.gov</t>
+  </si>
+  <si>
+    <t>NVDWR_Allocation All</t>
+  </si>
+  <si>
+    <t>Unspecified</t>
+  </si>
+  <si>
+    <t>NVDWR_Diversion Tracking</t>
+  </si>
+  <si>
+    <t>1) Added the following terms to CVs.SiteType: Storage, Other Surface Water,Geothermal, Other Ground Water, Effluent.</t>
+  </si>
+  <si>
+    <t>2) Added the following terms to the CVs.LegalStatus: Abrogated, Canceled, Certificate, Decreed, Ready For Action, Ready for Action (Protested), Relinquish a Portion, Relinquished, Reserved, Revocable Permit, Supersceded, Vested Rights</t>
   </si>
 </sst>
 </file>
@@ -892,7 +910,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1119,6 +1137,14 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1682,7 +1708,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1864,9 +1890,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1946,11 +1969,17 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="42" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2308,55 +2337,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="78" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="77" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="79" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="77" t="s">
         <v>244</v>
       </c>
       <c r="B1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="78" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="77" t="s">
         <v>245</v>
       </c>
       <c r="B2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="78" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="77" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7" s="67" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="66" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B8" s="67" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="66" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="78" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="77" t="s">
         <v>247</v>
       </c>
       <c r="B13" t="s">
         <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="91" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B15" s="91" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2369,32 +2408,32 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H8" sqref="H8:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="70.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="5"/>
+    <col min="11" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14"/>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -2426,7 +2465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2454,11 +2493,11 @@
       <c r="I3" s="17">
         <v>11</v>
       </c>
-      <c r="J3" s="69" t="s">
+      <c r="J3" s="68" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -2471,22 +2510,26 @@
       <c r="D4" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="62" t="s">
-        <v>254</v>
-      </c>
-      <c r="F4" s="46"/>
-      <c r="G4" s="47"/>
+      <c r="E4" s="61" t="s">
+        <v>284</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>39</v>
+      </c>
       <c r="H4" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="J4" s="69" t="s">
+      <c r="J4" s="68" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -2502,19 +2545,23 @@
       <c r="E5" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
+      <c r="F5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H5" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="J5" s="69" t="s">
+      <c r="J5" s="68" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -2530,19 +2577,23 @@
       <c r="E6" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+      <c r="F6" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="77">
+      <c r="I6" s="76">
         <v>0.5</v>
       </c>
-      <c r="J6" s="69" t="s">
+      <c r="J6" s="68" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -2558,19 +2609,23 @@
       <c r="E7" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
+      <c r="F7" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H7" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="69" t="s">
+      <c r="J7" s="68" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -2586,19 +2641,23 @@
       <c r="E8" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+      <c r="F8" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H8" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I8" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="J8" s="69" t="s">
+      <c r="J8" s="68" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -2614,17 +2673,21 @@
       <c r="E9" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+      <c r="F9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H9" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I9" s="18"/>
-      <c r="J9" s="69" t="s">
+      <c r="J9" s="68" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -2640,19 +2703,23 @@
       <c r="E10" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="F10" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H10" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="J10" s="69" t="s">
+      <c r="J10" s="68" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2665,22 +2732,26 @@
       <c r="D11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="79" t="s">
+      <c r="E11" s="78" t="s">
         <v>256</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
+      <c r="F11" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H11" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="J11" s="69" t="s">
+      <c r="J11" s="68" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -2696,20 +2767,24 @@
       <c r="E12" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
+      <c r="F12" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H12" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="J12" s="69" t="s">
+      <c r="J12" s="68" t="s">
         <v>223</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A18:A26">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:A26">
     <sortCondition ref="A18:A26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2721,33 +2796,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F86677-A939-4892-ADA0-492C09897DFD}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="93.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="5"/>
+    <col min="11" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -2779,7 +2854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -2807,11 +2882,11 @@
       <c r="I3" s="17">
         <v>16</v>
       </c>
-      <c r="J3" s="69" t="s">
+      <c r="J3" s="68" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>33</v>
       </c>
@@ -2825,7 +2900,7 @@
         <v>39</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="F4" s="46" t="s">
         <v>39</v>
@@ -2839,11 +2914,11 @@
       <c r="I4" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="J4" s="69" t="s">
+      <c r="J4" s="68" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -2859,19 +2934,23 @@
       <c r="E5" s="17">
         <v>1</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
+      <c r="F5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H5" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="17">
         <v>1</v>
       </c>
-      <c r="J5" s="69" t="s">
+      <c r="J5" s="68" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -2887,19 +2966,23 @@
       <c r="E6" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+      <c r="F6" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H6" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="J6" s="69" t="s">
+      <c r="J6" s="68" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
@@ -2915,19 +2998,23 @@
       <c r="E7" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
+      <c r="F7" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H7" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="J7" s="69" t="s">
+      <c r="J7" s="68" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -2943,19 +3030,23 @@
       <c r="E8" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+      <c r="F8" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H8" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I8" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="J8" s="69" t="s">
+      <c r="J8" s="68" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -2971,19 +3062,23 @@
       <c r="E9" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+      <c r="F9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H9" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I9" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="J9" s="69" t="s">
+      <c r="J9" s="68" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
@@ -2999,19 +3094,23 @@
       <c r="E10" s="17">
         <v>10</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="F10" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H10" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I10" s="17">
         <v>10</v>
       </c>
-      <c r="J10" s="69" t="s">
+      <c r="J10" s="68" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -3027,19 +3126,23 @@
       <c r="E11" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
+      <c r="F11" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H11" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="J11" s="69" t="s">
+      <c r="J11" s="68" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
@@ -3055,19 +3158,23 @@
       <c r="E12" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
+      <c r="F12" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H12" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="J12" s="69" t="s">
+      <c r="J12" s="68" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
@@ -3083,20 +3190,24 @@
       <c r="E13" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21"/>
+      <c r="F13" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H13" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I13" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="J13" s="69" t="s">
+      <c r="J13" s="68" t="s">
         <v>221</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A21:A30">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:A30">
     <sortCondition ref="A21:A30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3109,32 +3220,32 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F7" sqref="F7:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.1640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="20.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="60.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="5"/>
+    <col min="11" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -3166,7 +3277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>72</v>
       </c>
@@ -3194,11 +3305,11 @@
       <c r="I3" s="18">
         <v>1</v>
       </c>
-      <c r="J3" s="69" t="s">
+      <c r="J3" s="68" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>73</v>
       </c>
@@ -3226,11 +3337,11 @@
       <c r="I4" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="J4" s="69" t="s">
+      <c r="J4" s="68" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>79</v>
       </c>
@@ -3243,22 +3354,26 @@
       <c r="D5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="88" t="s">
+      <c r="E5" s="87" t="s">
         <v>281</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
+      <c r="F5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H5" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="J5" s="69" t="s">
+      <c r="J5" s="68" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>78</v>
       </c>
@@ -3274,19 +3389,23 @@
       <c r="E6" s="18" t="s">
         <v>280</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+      <c r="F6" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H6" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I6" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J6" s="69" t="s">
+      <c r="J6" s="68" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>80</v>
       </c>
@@ -3302,19 +3421,23 @@
       <c r="E7" s="89" t="s">
         <v>256</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
+      <c r="F7" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H7" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I7" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="J7" s="69" t="s">
+      <c r="J7" s="68" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>74</v>
       </c>
@@ -3330,19 +3453,23 @@
       <c r="E8" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+      <c r="F8" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H8" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I8" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="J8" s="69" t="s">
+      <c r="J8" s="68" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>77</v>
       </c>
@@ -3355,22 +3482,26 @@
       <c r="D9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="83" t="s">
+      <c r="E9" s="82" t="s">
         <v>261</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+      <c r="F9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H9" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I9" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="J9" s="69" t="s">
+      <c r="J9" s="68" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>75</v>
       </c>
@@ -3386,19 +3517,23 @@
       <c r="E10" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="F10" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H10" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="J10" s="69" t="s">
+      <c r="J10" s="68" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>76</v>
       </c>
@@ -3414,19 +3549,23 @@
       <c r="E11" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
+      <c r="F11" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H11" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="J11" s="69" t="s">
+      <c r="J11" s="68" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>81</v>
       </c>
@@ -3442,44 +3581,48 @@
       <c r="E12" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
+      <c r="F12" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H12" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="J12" s="69" t="s">
+      <c r="J12" s="68" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26"/>
     </row>
   </sheetData>
-  <sortState ref="A17:A25">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:A25">
     <sortCondition ref="A17:A25"/>
   </sortState>
   <hyperlinks>
@@ -3495,32 +3638,32 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.77734375" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="58.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="5"/>
+    <col min="11" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -3552,7 +3695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
@@ -3578,11 +3721,11 @@
       <c r="I3" s="17">
         <v>34658</v>
       </c>
-      <c r="J3" s="69" t="s">
+      <c r="J3" s="68" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>41</v>
       </c>
@@ -3598,17 +3741,21 @@
       <c r="E4" s="50" t="s">
         <v>268</v>
       </c>
-      <c r="F4" s="46"/>
-      <c r="G4" s="49"/>
+      <c r="F4" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="49" t="s">
+        <v>39</v>
+      </c>
       <c r="H4" s="19"/>
       <c r="I4" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="J4" s="69" t="s">
+      <c r="J4" s="68" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>47</v>
       </c>
@@ -3621,20 +3768,24 @@
       <c r="D5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="21"/>
+      <c r="F5" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H5" s="19"/>
       <c r="I5" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="69" t="s">
+      <c r="J5" s="68" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
@@ -3647,20 +3798,24 @@
       <c r="D6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="68" t="s">
+      <c r="E6" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="21"/>
+      <c r="F6" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H6" s="19"/>
       <c r="I6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="69" t="s">
+      <c r="J6" s="68" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>45</v>
       </c>
@@ -3673,20 +3828,24 @@
       <c r="D7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="21"/>
+      <c r="E7" s="90" t="s">
+        <v>283</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H7" s="19"/>
       <c r="I7" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="J7" s="69" t="s">
+      <c r="J7" s="68" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>43</v>
       </c>
@@ -3699,20 +3858,24 @@
       <c r="D8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="68" t="s">
+      <c r="E8" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="21"/>
+      <c r="F8" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H8" s="23"/>
       <c r="I8" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="J8" s="69" t="s">
+      <c r="J8" s="68" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>42</v>
       </c>
@@ -3725,20 +3888,24 @@
       <c r="D9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="68" t="s">
+      <c r="E9" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="21"/>
+      <c r="F9" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H9" s="19"/>
       <c r="I9" s="17">
         <v>17839</v>
       </c>
-      <c r="J9" s="69" t="s">
+      <c r="J9" s="68" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>44</v>
       </c>
@@ -3751,28 +3918,32 @@
       <c r="D10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="68" t="s">
-        <v>165</v>
-      </c>
-      <c r="F10" s="60"/>
-      <c r="G10" s="21"/>
+      <c r="E10" s="90" t="s">
+        <v>283</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H10" s="23"/>
       <c r="I10" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="J10" s="69" t="s">
+      <c r="J10" s="68" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C11" s="9"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C12" s="9"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C13" s="9"/>
     </row>
   </sheetData>
@@ -3786,32 +3957,32 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A20" sqref="A20:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.83203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="19.5" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="33.83203125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="73.1640625" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="5"/>
+    <col min="5" max="5" width="28.77734375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="33.77734375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="73.109375" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -3843,7 +4014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
@@ -3869,11 +4040,11 @@
       <c r="I3" s="18">
         <v>39035</v>
       </c>
-      <c r="J3" s="69" t="s">
+      <c r="J3" s="68" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>50</v>
       </c>
@@ -3887,17 +4058,21 @@
       <c r="E4" s="50" t="s">
         <v>269</v>
       </c>
-      <c r="F4" s="46"/>
-      <c r="G4" s="47"/>
+      <c r="F4" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>39</v>
+      </c>
       <c r="H4" s="19"/>
       <c r="I4" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="J4" s="69" t="s">
+      <c r="J4" s="68" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>59</v>
       </c>
@@ -3910,20 +4085,24 @@
       <c r="D5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="90" t="s">
         <v>119</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
+      <c r="F5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H5" s="19"/>
       <c r="I5" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="J5" s="69" t="s">
+      <c r="J5" s="68" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>58</v>
       </c>
@@ -3939,17 +4118,21 @@
       <c r="E6" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
+      <c r="F6" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="H6" s="19"/>
       <c r="I6" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="69" t="s">
+      <c r="J6" s="68" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>67</v>
       </c>
@@ -3962,8 +4145,12 @@
       <c r="D7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="E7" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>39</v>
+      </c>
       <c r="G7" s="27" t="s">
         <v>272</v>
       </c>
@@ -3971,11 +4158,11 @@
       <c r="I7" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="70" t="s">
+      <c r="J7" s="69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>61</v>
       </c>
@@ -4001,11 +4188,11 @@
       <c r="I8" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="J8" s="69" t="s">
+      <c r="J8" s="68" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -4018,16 +4205,22 @@
       <c r="D9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="27"/>
+      <c r="E9" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="H9" s="19"/>
       <c r="I9" s="18"/>
-      <c r="J9" s="69" t="s">
+      <c r="J9" s="68" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>60</v>
       </c>
@@ -4040,18 +4233,24 @@
       <c r="D10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
+      <c r="E10" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="H10" s="19"/>
       <c r="I10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="69" t="s">
+      <c r="J10" s="68" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>65</v>
       </c>
@@ -4064,8 +4263,12 @@
       <c r="D11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
+      <c r="E11" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>39</v>
+      </c>
       <c r="G11" s="27" t="s">
         <v>273</v>
       </c>
@@ -4073,11 +4276,11 @@
       <c r="I11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="70" t="s">
+      <c r="J11" s="69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>66</v>
       </c>
@@ -4090,18 +4293,24 @@
       <c r="D12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
+      <c r="E12" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="H12" s="19"/>
       <c r="I12" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="70" t="s">
+      <c r="J12" s="69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>56</v>
       </c>
@@ -4127,11 +4336,11 @@
       <c r="I13" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="J13" s="69" t="s">
+      <c r="J13" s="68" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
@@ -4157,11 +4366,11 @@
       <c r="I14" s="18">
         <v>-1067.700435</v>
       </c>
-      <c r="J14" s="69" t="s">
+      <c r="J14" s="68" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>62</v>
       </c>
@@ -4174,18 +4383,24 @@
       <c r="D15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27"/>
+      <c r="E15" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="H15" s="19"/>
       <c r="I15" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J15" s="69" t="s">
+      <c r="J15" s="68" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>63</v>
       </c>
@@ -4198,18 +4413,24 @@
       <c r="D16" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="27"/>
+      <c r="E16" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="H16" s="19"/>
       <c r="I16" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="69" t="s">
+      <c r="J16" s="68" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>52</v>
       </c>
@@ -4231,11 +4452,11 @@
       <c r="I17" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="J17" s="69" t="s">
+      <c r="J17" s="68" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>51</v>
       </c>
@@ -4248,18 +4469,24 @@
       <c r="D18" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="21"/>
+      <c r="E18" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="H18" s="23"/>
       <c r="I18" s="18">
         <v>3703994</v>
       </c>
-      <c r="J18" s="69" t="s">
+      <c r="J18" s="68" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>57</v>
       </c>
@@ -4272,18 +4499,24 @@
       <c r="D19" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="27"/>
+      <c r="E19" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="H19" s="19"/>
       <c r="I19" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="J19" s="70" t="s">
+      <c r="J19" s="69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>54</v>
       </c>
@@ -4296,7 +4529,9 @@
       <c r="D20" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="61"/>
+      <c r="E20" s="62" t="s">
+        <v>39</v>
+      </c>
       <c r="F20" s="26" t="s">
         <v>259</v>
       </c>
@@ -4307,11 +4542,11 @@
       <c r="I20" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="J20" s="69" t="s">
+      <c r="J20" s="68" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>64</v>
       </c>
@@ -4327,17 +4562,21 @@
       <c r="E21" s="26" t="s">
         <v>264</v>
       </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="27"/>
+      <c r="F21" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="H21" s="19"/>
       <c r="I21" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="J21" s="69" t="s">
+      <c r="J21" s="68" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>53</v>
       </c>
@@ -4350,19 +4589,25 @@
       <c r="D22" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27"/>
+      <c r="E22" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="H22" s="19"/>
       <c r="I22" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J22" s="70" t="s">
+      <c r="J22" s="69" t="s">
         <v>165</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A5:J26">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:J26">
     <sortCondition ref="A5:A26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4374,33 +4619,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="34.77734375" style="5" customWidth="1"/>
     <col min="2" max="2" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="5" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="116.1640625" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="5"/>
+    <col min="7" max="7" width="16.44140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="20.77734375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="116.109375" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -4432,7 +4677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="54" t="s">
         <v>82</v>
       </c>
@@ -4451,14 +4696,14 @@
       <c r="H3" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="71">
+      <c r="I3" s="70">
         <v>50004</v>
       </c>
-      <c r="J3" s="69" t="s">
+      <c r="J3" s="68" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="54" t="s">
         <v>6</v>
       </c>
@@ -4483,14 +4728,14 @@
       <c r="H4" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="71">
+      <c r="I4" s="70">
         <v>43</v>
       </c>
-      <c r="J4" s="69" t="s">
+      <c r="J4" s="68" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="54" t="s">
         <v>72</v>
       </c>
@@ -4515,14 +4760,14 @@
       <c r="H5" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="71">
+      <c r="I5" s="70">
         <v>1</v>
       </c>
-      <c r="J5" s="69" t="s">
+      <c r="J5" s="68" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="54" t="s">
         <v>49</v>
       </c>
@@ -4547,14 +4792,14 @@
       <c r="H6" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="71">
+      <c r="I6" s="70">
         <v>39035</v>
       </c>
-      <c r="J6" s="69" t="s">
+      <c r="J6" s="68" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="54" t="s">
         <v>23</v>
       </c>
@@ -4579,14 +4824,14 @@
       <c r="H7" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="71">
+      <c r="I7" s="70">
         <v>63</v>
       </c>
-      <c r="J7" s="69" t="s">
+      <c r="J7" s="68" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="54" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="54" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="54" t="s">
         <v>40</v>
       </c>
@@ -4611,14 +4856,14 @@
       <c r="H8" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="71">
+      <c r="I8" s="70">
         <v>371091</v>
       </c>
-      <c r="J8" s="69" t="s">
+      <c r="J8" s="68" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="54" t="s">
         <v>7</v>
       </c>
@@ -4631,22 +4876,26 @@
       <c r="D9" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="87" t="s">
+      <c r="E9" s="86" t="s">
         <v>254</v>
       </c>
-      <c r="F9" s="81"/>
-      <c r="G9" s="82"/>
+      <c r="F9" s="80" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="81" t="s">
+        <v>39</v>
+      </c>
       <c r="H9" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="69" t="s">
+      <c r="I9" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="68" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>73</v>
       </c>
@@ -4659,22 +4908,26 @@
       <c r="D10" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="84" t="s">
+      <c r="E10" s="83" t="s">
         <v>259</v>
       </c>
-      <c r="F10" s="60"/>
-      <c r="G10" s="27"/>
+      <c r="F10" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="H10" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="69" t="s">
+      <c r="I10" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="68" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>50</v>
       </c>
@@ -4687,22 +4940,26 @@
       <c r="D11" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="84" t="s">
+      <c r="E11" s="83" t="s">
         <v>269</v>
       </c>
-      <c r="F11" s="60"/>
-      <c r="G11" s="27"/>
+      <c r="F11" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="H11" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="69" t="s">
+      <c r="I11" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="68" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
@@ -4715,22 +4972,26 @@
       <c r="D12" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="85" t="s">
+      <c r="E12" s="84" t="s">
         <v>258</v>
       </c>
-      <c r="F12" s="60"/>
-      <c r="G12" s="27"/>
+      <c r="F12" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="H12" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="69" t="s">
+      <c r="I12" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="68" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>41</v>
       </c>
@@ -4743,22 +5004,26 @@
       <c r="D13" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="86" t="s">
+      <c r="E13" s="85" t="s">
         <v>249</v>
       </c>
-      <c r="F13" s="46"/>
-      <c r="G13" s="45"/>
+      <c r="F13" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="45" t="s">
+        <v>39</v>
+      </c>
       <c r="H13" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="69" t="s">
+      <c r="I13" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="68" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
@@ -4771,7 +5036,9 @@
       <c r="D14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="26"/>
+      <c r="E14" s="26" t="s">
+        <v>39</v>
+      </c>
       <c r="F14" s="36" t="s">
         <v>259</v>
       </c>
@@ -4784,11 +5051,11 @@
       <c r="I14" s="18">
         <v>1</v>
       </c>
-      <c r="J14" s="69" t="s">
+      <c r="J14" s="68" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="54" t="s">
         <v>153</v>
       </c>
@@ -4801,20 +5068,26 @@
       <c r="D15" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="51"/>
+      <c r="E15" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H15" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="71">
+      <c r="I15" s="70">
         <v>5363</v>
       </c>
-      <c r="J15" s="69" t="s">
+      <c r="J15" s="68" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>96</v>
       </c>
@@ -4827,20 +5100,26 @@
       <c r="D16" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="51"/>
+      <c r="E16" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H16" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I16" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J16" s="70" t="s">
+      <c r="J16" s="69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>95</v>
       </c>
@@ -4853,20 +5132,26 @@
       <c r="D17" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="51"/>
+      <c r="E17" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H17" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I17" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J17" s="70" t="s">
+      <c r="J17" s="69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="39" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="54" t="s">
         <v>86</v>
       </c>
@@ -4879,20 +5164,26 @@
       <c r="D18" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="21"/>
+      <c r="E18" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H18" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I18" s="71" t="s">
+      <c r="I18" s="70" t="s">
         <v>158</v>
       </c>
-      <c r="J18" s="69" t="s">
+      <c r="J18" s="68" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>97</v>
       </c>
@@ -4905,20 +5196,26 @@
       <c r="D19" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="51"/>
+      <c r="E19" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H19" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I19" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="J19" s="70" t="s">
+      <c r="J19" s="69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>94</v>
       </c>
@@ -4931,20 +5228,26 @@
       <c r="D20" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="26"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="51"/>
+      <c r="E20" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H20" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I20" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="J20" s="69" t="s">
+      <c r="J20" s="68" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>89</v>
       </c>
@@ -4957,20 +5260,26 @@
       <c r="D21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="21"/>
+      <c r="E21" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H21" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I21" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="J21" s="70" t="s">
+      <c r="I21" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" s="69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>155</v>
       </c>
@@ -4983,20 +5292,26 @@
       <c r="D22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="26"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="21"/>
+      <c r="E22" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H22" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I22" s="18">
         <v>5200</v>
       </c>
-      <c r="J22" s="69" t="s">
+      <c r="J22" s="68" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
@@ -5009,7 +5324,9 @@
       <c r="D23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="66"/>
+      <c r="E23" s="65" t="s">
+        <v>39</v>
+      </c>
       <c r="F23" s="36" t="s">
         <v>259</v>
       </c>
@@ -5022,11 +5339,11 @@
       <c r="I23" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="J23" s="69" t="s">
+      <c r="J23" s="68" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>90</v>
       </c>
@@ -5039,20 +5356,26 @@
       <c r="D24" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="21"/>
+      <c r="E24" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H24" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I24" s="18">
         <v>0</v>
       </c>
-      <c r="J24" s="69" t="s">
+      <c r="J24" s="68" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>84</v>
       </c>
@@ -5065,7 +5388,9 @@
       <c r="D25" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="26"/>
+      <c r="E25" s="26" t="s">
+        <v>39</v>
+      </c>
       <c r="F25" s="36" t="s">
         <v>259</v>
       </c>
@@ -5078,11 +5403,11 @@
       <c r="I25" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="J25" s="69" t="s">
+      <c r="J25" s="68" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>85</v>
       </c>
@@ -5095,8 +5420,12 @@
       <c r="D26" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="63"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>39</v>
+      </c>
       <c r="G26" s="21"/>
       <c r="H26" s="40" t="s">
         <v>39</v>
@@ -5104,11 +5433,11 @@
       <c r="I26" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="J26" s="69" t="s">
+      <c r="J26" s="68" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>154</v>
       </c>
@@ -5121,8 +5450,12 @@
       <c r="D27" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="26"/>
-      <c r="F27" s="36"/>
+      <c r="E27" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>39</v>
+      </c>
       <c r="G27" s="21" t="s">
         <v>275</v>
       </c>
@@ -5132,11 +5465,11 @@
       <c r="I27" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="J27" s="69" t="s">
+      <c r="J27" s="68" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" s="39" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>156</v>
       </c>
@@ -5149,20 +5482,26 @@
       <c r="D28" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="21"/>
+      <c r="E28" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H28" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I28" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="J28" s="69" t="s">
+      <c r="I28" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28" s="68" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>106</v>
       </c>
@@ -5175,22 +5514,26 @@
       <c r="D29" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="80">
+      <c r="E29" s="79">
         <v>44196</v>
       </c>
-      <c r="F29" s="36"/>
-      <c r="G29" s="21"/>
+      <c r="F29" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H29" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I29" s="74">
+      <c r="I29" s="73">
         <v>44196</v>
       </c>
-      <c r="J29" s="69" t="s">
+      <c r="J29" s="68" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>105</v>
       </c>
@@ -5203,22 +5546,26 @@
       <c r="D30" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="80">
+      <c r="E30" s="79">
         <v>43831</v>
       </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="21"/>
+      <c r="F30" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="H30" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I30" s="74">
+      <c r="I30" s="73">
         <v>43831</v>
       </c>
-      <c r="J30" s="69" t="s">
+      <c r="J30" s="68" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>88</v>
       </c>
@@ -5231,20 +5578,26 @@
       <c r="D31" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="66"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="21"/>
+      <c r="E31" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H31" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I31" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J31" s="70" t="s">
+      <c r="J31" s="69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>152</v>
       </c>
@@ -5257,7 +5610,9 @@
       <c r="D32" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="66"/>
+      <c r="E32" s="65" t="s">
+        <v>39</v>
+      </c>
       <c r="F32" s="36" t="s">
         <v>259</v>
       </c>
@@ -5267,14 +5622,14 @@
       <c r="H32" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I32" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="J32" s="69" t="s">
+      <c r="I32" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" s="68" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>103</v>
       </c>
@@ -5287,20 +5642,26 @@
       <c r="D33" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="26"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="21"/>
+      <c r="E33" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F33" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H33" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I33" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J33" s="70" t="s">
+      <c r="J33" s="69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>100</v>
       </c>
@@ -5313,20 +5674,26 @@
       <c r="D34" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="26"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="21"/>
+      <c r="E34" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F34" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H34" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I34" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J34" s="69" t="s">
+      <c r="J34" s="68" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="54" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" s="54" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>102</v>
       </c>
@@ -5339,20 +5706,26 @@
       <c r="D35" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="26"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="21"/>
+      <c r="E35" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F35" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H35" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I35" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J35" s="69" t="s">
+      <c r="J35" s="68" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="54" t="s">
         <v>157</v>
       </c>
@@ -5365,22 +5738,26 @@
       <c r="D36" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="65"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="90">
+      <c r="E36" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" s="88">
         <v>44032</v>
       </c>
       <c r="H36" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I36" s="75">
+      <c r="I36" s="74">
         <v>43874</v>
       </c>
-      <c r="J36" s="69" t="s">
+      <c r="J36" s="68" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>83</v>
       </c>
@@ -5393,20 +5770,26 @@
       <c r="D37" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="26"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="21"/>
+      <c r="E37" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F37" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H37" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I37" s="76">
+      <c r="I37" s="75">
         <v>33187</v>
       </c>
-      <c r="J37" s="70" t="s">
+      <c r="J37" s="69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>92</v>
       </c>
@@ -5419,20 +5802,26 @@
       <c r="D38" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="26"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="21"/>
+      <c r="E38" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H38" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I38" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="J38" s="69" t="s">
+      <c r="I38" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="J38" s="68" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>93</v>
       </c>
@@ -5445,18 +5834,24 @@
       <c r="D39" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="26"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="21"/>
+      <c r="E39" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H39" s="39"/>
-      <c r="I39" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="J39" s="69" t="s">
+      <c r="I39" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="J39" s="68" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>101</v>
       </c>
@@ -5469,20 +5864,26 @@
       <c r="D40" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E40" s="26"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="21"/>
+      <c r="E40" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F40" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G40" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H40" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I40" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J40" s="69" t="s">
+      <c r="J40" s="68" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>98</v>
       </c>
@@ -5495,20 +5896,26 @@
       <c r="D41" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E41" s="26"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="21"/>
+      <c r="E41" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G41" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H41" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I41" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="J41" s="70" t="s">
+      <c r="I41" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="J41" s="69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>91</v>
       </c>
@@ -5521,20 +5928,26 @@
       <c r="D42" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="26"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="21"/>
+      <c r="E42" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F42" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G42" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H42" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I42" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="J42" s="69" t="s">
+      <c r="I42" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="J42" s="68" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>104</v>
       </c>
@@ -5547,20 +5960,26 @@
       <c r="D43" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E43" s="26"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="21"/>
+      <c r="E43" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G43" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H43" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I43" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J43" s="70" t="s">
+      <c r="J43" s="69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="54" t="s">
         <v>151</v>
       </c>
@@ -5573,20 +5992,26 @@
       <c r="D44" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="26"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="21"/>
+      <c r="E44" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F44" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G44" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="H44" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I44" s="71" t="s">
+      <c r="I44" s="70" t="s">
         <v>134</v>
       </c>
-      <c r="J44" s="69" t="s">
+      <c r="J44" s="68" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>99</v>
       </c>
@@ -5599,7 +6024,9 @@
       <c r="D45" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E45" s="26"/>
+      <c r="E45" s="26" t="s">
+        <v>39</v>
+      </c>
       <c r="F45" s="36" t="s">
         <v>259</v>
       </c>
@@ -5612,12 +6039,12 @@
       <c r="I45" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J45" s="69" t="s">
+      <c r="J45" s="68" t="s">
         <v>217</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A14:J45">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:J45">
     <sortCondition ref="A14:A45"/>
   </sortState>
   <phoneticPr fontId="25" type="noConversion"/>
@@ -5634,35 +6061,35 @@
       <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="64"/>
-      <c r="B3" s="64"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="64"/>
-      <c r="B5" s="64"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="64"/>
-      <c r="B6" s="64"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="64"/>
-      <c r="B7" s="64"/>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="63"/>
+      <c r="B5" s="63"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="63"/>
+      <c r="B6" s="63"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="63"/>
+      <c r="B7" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nevada update to files 09022020
Nevada update to files 09022020.
</commit_message>
<xml_diff>
--- a/Nevada/WaterAllocation/NV_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Nevada/WaterAllocation/NV_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Nevada\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BB6AD9-6048-4E79-BA9E-E0D658AFDA9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DB3C53-A6F3-42C6-B808-4AE49AD13037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="714" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Sites" sheetId="5" r:id="rId6"/>
     <sheet name="AllocationsAmounts_fact" sheetId="7" r:id="rId7"/>
     <sheet name="BeneficialUseCategory" sheetId="9" r:id="rId8"/>
+    <sheet name="Misc" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="316">
   <si>
     <t>AllocationAmount</t>
   </si>
@@ -901,6 +902,93 @@
   </si>
   <si>
     <t>2) Added the following terms to the CVs.LegalStatus: Abrogated, Canceled, Certificate, Decreed, Ready For Action, Ready for Action (Protested), Relinquish a Portion, Relinquished, Reserved, Revocable Permit, Supersceded, Vested Rights</t>
+  </si>
+  <si>
+    <t>Looks like there x &amp; y or the lat &amp; long are already in a good format for us to use, no need to conver.</t>
+  </si>
+  <si>
+    <t>their linking elementat between sheets appears to be the 'app' field.</t>
+  </si>
+  <si>
+    <t>mixed up sitetype and watersourcetype, could probalby fix.  Can make a custom sitetype list that gets into the water soruce type (surface v gound), where the watersource gets into specifics (lake, river, well, etc).</t>
+  </si>
+  <si>
+    <t>owner_name</t>
+  </si>
+  <si>
+    <t>EFF</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>Effluent</t>
+  </si>
+  <si>
+    <t>GEO</t>
+  </si>
+  <si>
+    <t>Geothermal</t>
+  </si>
+  <si>
+    <t>LAK</t>
+  </si>
+  <si>
+    <t>lake</t>
+  </si>
+  <si>
+    <t>OGW</t>
+  </si>
+  <si>
+    <t>Other Ground Water</t>
+  </si>
+  <si>
+    <t>OSW</t>
+  </si>
+  <si>
+    <t>Other Surface Water</t>
+  </si>
+  <si>
+    <t>RES</t>
+  </si>
+  <si>
+    <t>Reservoir</t>
+  </si>
+  <si>
+    <t>SPR</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>STO</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>stream</t>
+  </si>
+  <si>
+    <t>UG</t>
+  </si>
+  <si>
+    <t>Underground</t>
+  </si>
+  <si>
+    <t>UKN</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Groundwater</t>
+  </si>
+  <si>
+    <t>Reuse</t>
   </si>
 </sst>
 </file>
@@ -910,7 +998,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1148,6 +1236,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1708,7 +1801,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1981,6 +2074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2337,10 +2431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2396,6 +2490,21 @@
     <row r="15" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="91" t="s">
         <v>286</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -3638,7 +3747,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3956,8 +4065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E7F0DF-14BE-4BB8-BB6C-8815808B0B66}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:E20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="A14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4619,8 +4728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5424,9 +5533,11 @@
         <v>39</v>
       </c>
       <c r="F26" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" s="21"/>
+        <v>259</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>290</v>
+      </c>
       <c r="H26" s="40" t="s">
         <v>39</v>
       </c>
@@ -6094,4 +6205,221 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5DE272-04F8-4611-B79A-B07C0092FE3A}">
+  <dimension ref="B1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E1" s="92" t="s">
+        <v>315</v>
+      </c>
+      <c r="G1" t="str">
+        <f>""""&amp;B1&amp;""""&amp;" : "&amp;""""&amp;E1&amp;""""&amp;","</f>
+        <v>"EFF" : "Reuse",</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G11" si="0">""""&amp;B2&amp;""""&amp;" : "&amp;""""&amp;E2&amp;""""&amp;","</f>
+        <v>"GEO" : "Groundwater",</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E3" s="92" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>"LAK" : "Surface Water",</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E4" s="92" t="s">
+        <v>314</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>"OGW" : "Groundwater",</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D5" t="s">
+        <v>301</v>
+      </c>
+      <c r="E5" s="92" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>"OSW" : "Surface Water",</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D6" t="s">
+        <v>303</v>
+      </c>
+      <c r="E6" t="s">
+        <v>303</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>"RES" : "Reservoir",</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D7" t="s">
+        <v>305</v>
+      </c>
+      <c r="E7" s="92" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>"SPR" : "Surface Water",</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>306</v>
+      </c>
+      <c r="C8" t="s">
+        <v>292</v>
+      </c>
+      <c r="D8" t="s">
+        <v>307</v>
+      </c>
+      <c r="E8" t="s">
+        <v>307</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>"STO" : "Storage",</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>308</v>
+      </c>
+      <c r="C9" t="s">
+        <v>292</v>
+      </c>
+      <c r="D9" t="s">
+        <v>309</v>
+      </c>
+      <c r="E9" s="92" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>"STR" : "Surface Water",</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>310</v>
+      </c>
+      <c r="C10" t="s">
+        <v>292</v>
+      </c>
+      <c r="D10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E10" s="92" t="s">
+        <v>314</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>"UG" : "Groundwater",</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>312</v>
+      </c>
+      <c r="C11" t="s">
+        <v>292</v>
+      </c>
+      <c r="D11" t="s">
+        <v>313</v>
+      </c>
+      <c r="E11" s="92" t="s">
+        <v>119</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>"UKN" : "Unknown",</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Nevada water rights update
Nevada water rights update
</commit_message>
<xml_diff>
--- a/Nevada/WaterAllocation/NV_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Nevada/WaterAllocation/NV_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Nevada\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DB3C53-A6F3-42C6-B808-4AE49AD13037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A89F29F-F3A5-432D-9568-53F80419F485}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="714" activeTab="5" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="318">
   <si>
     <t>AllocationAmount</t>
   </si>
@@ -989,6 +989,12 @@
   </si>
   <si>
     <t>Reuse</t>
+  </si>
+  <si>
+    <t>Create Custom WaDE Water Source ID</t>
+  </si>
+  <si>
+    <t>Create Custom WaDE Site ID</t>
   </si>
 </sst>
 </file>
@@ -1801,7 +1807,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2075,6 +2081,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3746,8 +3755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC5F405-0A84-4CAE-BAB0-9DF044EAE9B9}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3984,7 +3993,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>42</v>
       </c>
@@ -3997,8 +4006,8 @@
       <c r="D9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="67" t="s">
-        <v>165</v>
+      <c r="E9" s="93" t="s">
+        <v>316</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>39</v>
@@ -4065,8 +4074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E7F0DF-14BE-4BB8-BB6C-8815808B0B66}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="A14:G14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4578,8 +4587,8 @@
       <c r="D18" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="26" t="s">
-        <v>163</v>
+      <c r="E18" s="93" t="s">
+        <v>317</v>
       </c>
       <c r="F18" s="26" t="s">
         <v>39</v>
@@ -4728,8 +4737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>